<commit_message>
SOL is very difficult in some data/seasons, looking at nest meaures
</commit_message>
<xml_diff>
--- a/export/T_SOL_summary_All.xlsx
+++ b/export/T_SOL_summary_All.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="150">
   <si>
     <t>Description</t>
   </si>
@@ -193,6 +193,276 @@
   </si>
   <si>
     <t>-80.38 ± 92.78</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>44.57 ± 29.38</t>
+  </si>
+  <si>
+    <t>12.98 ± 70.52</t>
+  </si>
+  <si>
+    <t>73.58 ± 100.07</t>
+  </si>
+  <si>
+    <t>-66.96 ± 90.81</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>44.37 ± 31.01</t>
+  </si>
+  <si>
+    <t>53.26 ± 74.03</t>
+  </si>
+  <si>
+    <t>106.51 ± 121.88</t>
+  </si>
+  <si>
+    <t>-135.76 ± 111.81</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>38.34 ± 40.30</t>
+  </si>
+  <si>
+    <t>62.81 ± 94.60</t>
+  </si>
+  <si>
+    <t>94.65 ± 114.80</t>
+  </si>
+  <si>
+    <t>-100.03 ± 90.53</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>32.71 ± 22.29</t>
+  </si>
+  <si>
+    <t>-15.18 ± 26.14</t>
+  </si>
+  <si>
+    <t>62.76 ± 76.36</t>
+  </si>
+  <si>
+    <t>-25.07 ± 57.46</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>40.43 ± 32.48</t>
+  </si>
+  <si>
+    <t>30.66 ± 79.46</t>
+  </si>
+  <si>
+    <t>84.69 ± 106.87</t>
+  </si>
+  <si>
+    <t>-83.27 ± 97.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>44.57 ± 29.38</t>
+  </si>
+  <si>
+    <t>12.98 ± 70.52</t>
+  </si>
+  <si>
+    <t>73.58 ± 100.07</t>
+  </si>
+  <si>
+    <t>-66.96 ± 90.81</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>44.37 ± 31.01</t>
+  </si>
+  <si>
+    <t>53.26 ± 74.03</t>
+  </si>
+  <si>
+    <t>106.51 ± 121.88</t>
+  </si>
+  <si>
+    <t>-135.76 ± 111.81</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>38.34 ± 40.30</t>
+  </si>
+  <si>
+    <t>62.81 ± 94.60</t>
+  </si>
+  <si>
+    <t>94.65 ± 114.80</t>
+  </si>
+  <si>
+    <t>-100.03 ± 90.53</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>32.71 ± 22.29</t>
+  </si>
+  <si>
+    <t>-15.18 ± 26.14</t>
+  </si>
+  <si>
+    <t>62.76 ± 76.36</t>
+  </si>
+  <si>
+    <t>-25.07 ± 57.46</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>40.43 ± 32.48</t>
+  </si>
+  <si>
+    <t>30.66 ± 79.46</t>
+  </si>
+  <si>
+    <t>84.69 ± 106.87</t>
+  </si>
+  <si>
+    <t>-83.27 ± 97.97</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Latency to AB</t>
+  </si>
+  <si>
+    <t>AB Rel. to Sunrise</t>
+  </si>
+  <si>
+    <t>Latency to QB</t>
+  </si>
+  <si>
+    <t>QB Rel. to Sunset</t>
+  </si>
+  <si>
+    <t>Winter</t>
+  </si>
+  <si>
+    <t>44.14 ± 27.69</t>
+  </si>
+  <si>
+    <t>13.93 ± 70.73</t>
+  </si>
+  <si>
+    <t>74.90 ± 101.84</t>
+  </si>
+  <si>
+    <t>-66.68 ± 90.98</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>45.05 ± 29.54</t>
+  </si>
+  <si>
+    <t>51.57 ± 73.87</t>
+  </si>
+  <si>
+    <t>98.65 ± 115.50</t>
+  </si>
+  <si>
+    <t>-122.99 ± 99.87</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t>33.17 ± 33.61</t>
+  </si>
+  <si>
+    <t>58.76 ± 67.73</t>
+  </si>
+  <si>
+    <t>83.01 ± 96.36</t>
+  </si>
+  <si>
+    <t>-80.22 ± 76.16</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>28.89 ± 14.31</t>
+  </si>
+  <si>
+    <t>-12.00 ± 22.93</t>
+  </si>
+  <si>
+    <t>55.06 ± 64.13</t>
+  </si>
+  <si>
+    <t>-22.75 ± 55.94</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>39.52 ± 28.68</t>
+  </si>
+  <si>
+    <t>28.20 ± 70.47</t>
+  </si>
+  <si>
+    <t>78.94 ± 99.99</t>
+  </si>
+  <si>
+    <t>-75.51 ± 91.07</t>
   </si>
 </sst>
 </file>
@@ -213,7 +483,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -223,14 +493,20 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -244,8 +520,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="true"/>
-    <col min="2" max="2" width="12.140625" customWidth="true"/>
-    <col min="3" max="3" width="14.140625" customWidth="true"/>
+    <col min="2" max="2" width="13.140625" customWidth="true"/>
+    <col min="3" max="3" width="13.140625" customWidth="true"/>
     <col min="4" max="4" width="12.140625" customWidth="true"/>
     <col min="5" max="5" width="12.85546875" customWidth="true"/>
     <col min="6" max="6" width="12.140625" customWidth="true"/>
@@ -253,102 +529,102 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>55</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>51</v>
+        <v>141</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>56</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>37</v>
+        <v>127</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>57</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>48</v>
+        <v>138</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>53</v>
+        <v>143</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>58</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>44</v>
+        <v>134</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>54</v>
+        <v>144</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>59</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>